<commit_message>
resolved discrepancies between visit and encounterDatetime
</commit_message>
<xml_diff>
--- a/LAMIS-NMRS/Templates/NMRSRegimen.xlsx
+++ b/LAMIS-NMRS/Templates/NMRSRegimen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hvalentine\Documents\GitHub\LAMIS-NMRS\LAMIS-NMRS\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hvalentine\Documents\GitHub\emr-migration\LAMIS-NMRS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3392B3BA-BCEE-4EA0-A500-89B55A2DAE69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2349D07B-7266-4DB8-9366-B27246C8B7D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{814E9652-A163-4A47-8883-35DF14B93540}"/>
   </bookViews>
@@ -642,7 +642,7 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1273,7 +1273,9 @@
       <c r="F27" s="1">
         <v>164513</v>
       </c>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1">
+        <v>165523</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
@@ -1340,7 +1342,9 @@
       <c r="F30" s="1">
         <v>164513</v>
       </c>
-      <c r="G30" s="1"/>
+      <c r="G30" s="1">
+        <v>165534</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">

</xml_diff>